<commit_message>
2 baskets method implemented
</commit_message>
<xml_diff>
--- a/poverty_measurement/input/canastapercapita_metocol_sin_outliars.xlsx
+++ b/poverty_measurement/input/canastapercapita_metocol_sin_outliars.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="80">
   <si>
     <t>bien</t>
   </si>
@@ -21,6 +21,12 @@
     <t>Arroz, harina de arroz</t>
   </si>
   <si>
+    <t>Avena, avena en hojuelas, harina de avena</t>
+  </si>
+  <si>
+    <t>Galletas, dulces, saladas, integrales</t>
+  </si>
+  <si>
     <t>Harina de maiz</t>
   </si>
   <si>
@@ -33,21 +39,69 @@
     <t>Pastas alimenticias</t>
   </si>
   <si>
+    <t>Fororo</t>
+  </si>
+  <si>
+    <t>Otro (especifique)</t>
+  </si>
+  <si>
     <t>Carne de res (bistec, carne molida, carne para esmechar)</t>
   </si>
   <si>
+    <t>Visceras (higado, riñonada, corazon, asadura, morcillas)</t>
+  </si>
+  <si>
+    <t>Chuleta de cerdo ahumada</t>
+  </si>
+  <si>
+    <t>Carne de cerdo fresca (chuleta, costilla, pernil)</t>
+  </si>
+  <si>
+    <t>Hueso de res, pata de res, pata de pollo</t>
+  </si>
+  <si>
+    <t>Chorizo, jamon, mortadela y otros embutidos</t>
+  </si>
+  <si>
+    <t>Carne enlatada</t>
+  </si>
+  <si>
     <t>Carne de pollo</t>
   </si>
   <si>
+    <t>Pescado enlatado</t>
+  </si>
+  <si>
+    <t>Sardinas frescas/congeladas</t>
+  </si>
+  <si>
+    <t>Atun fresco/congelado</t>
+  </si>
+  <si>
     <t>Pescado fresco</t>
   </si>
   <si>
+    <t>Pescado seco/salado</t>
+  </si>
+  <si>
+    <t>Leche liquida, completa o descremada</t>
+  </si>
+  <si>
     <t>Leche en polvo, completa o descremada</t>
   </si>
   <si>
+    <t>Queso requeson, ricota</t>
+  </si>
+  <si>
     <t>Queso blanco</t>
   </si>
   <si>
+    <t>Queso amarillo</t>
+  </si>
+  <si>
+    <t>Suero, natilla, nata</t>
+  </si>
+  <si>
     <t>Huevos (unidades)</t>
   </si>
   <si>
@@ -63,18 +117,42 @@
     <t>Cambur</t>
   </si>
   <si>
+    <t>Mangos</t>
+  </si>
+  <si>
     <t>Platanos</t>
   </si>
   <si>
+    <t>Lechosa</t>
+  </si>
+  <si>
+    <t>Guayaba</t>
+  </si>
+  <si>
     <t>Tomates</t>
   </si>
   <si>
+    <t>Aguacate</t>
+  </si>
+  <si>
     <t>Aji dulce, pimenton, pimiento</t>
   </si>
   <si>
     <t>Cebolla</t>
   </si>
   <si>
+    <t>Auyama</t>
+  </si>
+  <si>
+    <t>Lechuga</t>
+  </si>
+  <si>
+    <t>Berenjena</t>
+  </si>
+  <si>
+    <t>Zanahorias</t>
+  </si>
+  <si>
     <t>Cebollin, ajoporro, cilantro y similares</t>
   </si>
   <si>
@@ -87,19 +165,82 @@
     <t>Lentejas</t>
   </si>
   <si>
+    <t>Garbanzo</t>
+  </si>
+  <si>
+    <t>Nueces</t>
+  </si>
+  <si>
+    <t>Mani</t>
+  </si>
+  <si>
+    <t>Merey</t>
+  </si>
+  <si>
     <t>Yuca</t>
   </si>
   <si>
     <t>Papas</t>
   </si>
   <si>
+    <t>Ocumo</t>
+  </si>
+  <si>
+    <t>Apio</t>
+  </si>
+  <si>
+    <t>Casabe</t>
+  </si>
+  <si>
     <t>Azucar</t>
   </si>
   <si>
+    <t>Papelon</t>
+  </si>
+  <si>
+    <t>Edulcorantes</t>
+  </si>
+  <si>
+    <t>Miel</t>
+  </si>
+  <si>
+    <t>Melaza</t>
+  </si>
+  <si>
     <t>Cafe</t>
   </si>
   <si>
+    <t>Te</t>
+  </si>
+  <si>
+    <t>Bebida achocolatada</t>
+  </si>
+  <si>
     <t>Sal</t>
+  </si>
+  <si>
+    <t>Concentrados (cubitos, sopas de sobre)</t>
+  </si>
+  <si>
+    <t>Salsa de tomate</t>
+  </si>
+  <si>
+    <t>Otras salsas</t>
+  </si>
+  <si>
+    <t>Jugos</t>
+  </si>
+  <si>
+    <t>Agua embotellada</t>
+  </si>
+  <si>
+    <t>Gaseosas/refrescos</t>
+  </si>
+  <si>
+    <t>Otras bebidas no alcoholicas</t>
+  </si>
+  <si>
+    <t>Bebidas alcoholicas</t>
   </si>
   <si>
     <t>cantidad_ajustada</t>
@@ -157,7 +298,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E89"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -165,16 +306,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>76</v>
       </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>77</v>
       </c>
       <c r="D1" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="E1" t="s">
-        <v>32</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2">
@@ -199,16 +340,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>125.63386194155223</v>
+        <v>0</v>
       </c>
       <c r="C3" s="1">
         <v>4723</v>
       </c>
       <c r="D3" s="1">
-        <v>3.8299999237060547</v>
+        <v>4.125</v>
       </c>
       <c r="E3" s="1">
-        <v>481.17767333984375</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -216,16 +357,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>18.338965379810677</v>
+        <v>0</v>
       </c>
       <c r="C4" s="1">
         <v>4723</v>
       </c>
       <c r="D4" s="1">
-        <v>3.5499999523162842</v>
+        <v>4.5275001525878906</v>
       </c>
       <c r="E4" s="1">
-        <v>65.103324890136719</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -233,16 +374,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>1.8439675338586812</v>
+        <v>125.63386194155223</v>
       </c>
       <c r="C5" s="1">
         <v>4723</v>
       </c>
       <c r="D5" s="1">
-        <v>2.8466665744781494</v>
+        <v>3.8299999237060547</v>
       </c>
       <c r="E5" s="1">
-        <v>5.2491607666015625</v>
+        <v>481.17767333984375</v>
       </c>
     </row>
     <row r="6">
@@ -250,16 +391,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>57.066627874784288</v>
+        <v>18.338965379810677</v>
       </c>
       <c r="C6" s="1">
         <v>4723</v>
       </c>
       <c r="D6" s="1">
-        <v>1.375</v>
+        <v>3.5499999523162842</v>
       </c>
       <c r="E6" s="1">
-        <v>78.46661376953125</v>
+        <v>65.103324890136719</v>
       </c>
     </row>
     <row r="7">
@@ -267,16 +408,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>35.773522600541042</v>
+        <v>1.8439675338586812</v>
       </c>
       <c r="C7" s="1">
         <v>4723</v>
       </c>
       <c r="D7" s="1">
-        <v>1.9650000333786011</v>
+        <v>2.8466665744781494</v>
       </c>
       <c r="E7" s="1">
-        <v>70.294975280761719</v>
+        <v>5.2491607666015625</v>
       </c>
     </row>
     <row r="8">
@@ -284,16 +425,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>20.380797466937956</v>
+        <v>57.066627874784288</v>
       </c>
       <c r="C8" s="1">
         <v>4723</v>
       </c>
       <c r="D8" s="1">
-        <v>1.7400000095367432</v>
+        <v>1.375</v>
       </c>
       <c r="E8" s="1">
-        <v>35.462589263916016</v>
+        <v>78.46661376953125</v>
       </c>
     </row>
     <row r="9">
@@ -301,16 +442,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>32.047278376572621</v>
+        <v>0</v>
       </c>
       <c r="C9" s="1">
         <v>4723</v>
       </c>
       <c r="D9" s="1">
-        <v>0.85000002384185791</v>
+        <v>3.7999999523162842</v>
       </c>
       <c r="E9" s="1">
-        <v>27.24018669128418</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -318,33 +459,29 @@
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>7.5887418317259705</v>
+        <v>0</v>
       </c>
       <c r="C10" s="1">
         <v>4723</v>
       </c>
-      <c r="D10" s="1">
-        <v>4.2849998474121094</v>
-      </c>
-      <c r="E10" s="1">
-        <v>32.517757415771484</v>
-      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
     </row>
     <row r="11">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>26.284929443713143</v>
+        <v>35.773522600541042</v>
       </c>
       <c r="C11" s="1">
         <v>4723</v>
       </c>
       <c r="D11" s="1">
-        <v>3.684999942779541</v>
+        <v>1.9650000333786011</v>
       </c>
       <c r="E11" s="1">
-        <v>96.859962463378906</v>
+        <v>70.294975280761719</v>
       </c>
     </row>
     <row r="12">
@@ -352,16 +489,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="1">
-        <v>21.167612287823033</v>
+        <v>0</v>
       </c>
       <c r="C12" s="1">
         <v>4723</v>
       </c>
       <c r="D12" s="1">
-        <v>1.4500000476837158</v>
+        <v>2.1766667366027832</v>
       </c>
       <c r="E12" s="1">
-        <v>30.693038940429688</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -369,16 +506,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="1">
-        <v>25.771581386954455</v>
+        <v>0</v>
       </c>
       <c r="C13" s="1">
         <v>4723</v>
       </c>
       <c r="D13" s="1">
-        <v>9</v>
+        <v>2.0099999904632568</v>
       </c>
       <c r="E13" s="1">
-        <v>231.94422912597656</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -386,16 +523,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="1">
-        <v>7.1381170796358608</v>
+        <v>0</v>
       </c>
       <c r="C14" s="1">
         <v>4723</v>
       </c>
       <c r="D14" s="1">
-        <v>5.8400001525878906</v>
+        <v>1.9199999570846558</v>
       </c>
       <c r="E14" s="1">
-        <v>41.686603546142578</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -403,16 +540,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="1">
-        <v>10.352916163835843</v>
+        <v>0</v>
       </c>
       <c r="C15" s="1">
         <v>4723</v>
       </c>
       <c r="D15" s="1">
-        <v>3.0799999237060547</v>
+        <v>1.8324999809265137</v>
       </c>
       <c r="E15" s="1">
-        <v>31.886980056762695</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -420,16 +557,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="1">
-        <v>39.938503641358324</v>
+        <v>0</v>
       </c>
       <c r="C16" s="1">
         <v>4723</v>
       </c>
       <c r="D16" s="1">
-        <v>1.1337499618530273</v>
+        <v>2.7799999713897705</v>
       </c>
       <c r="E16" s="1">
-        <v>45.280277252197266</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -437,16 +574,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="1">
-        <v>21.064435758960215</v>
+        <v>0</v>
       </c>
       <c r="C17" s="1">
         <v>4723</v>
       </c>
       <c r="D17" s="1">
-        <v>1.6485714912414551</v>
+        <v>2.2000000476837158</v>
       </c>
       <c r="E17" s="1">
-        <v>34.726226806640625</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -454,204 +591,1172 @@
         <v>17</v>
       </c>
       <c r="B18" s="1">
-        <v>11.258825547660328</v>
+        <v>20.380797466937956</v>
       </c>
       <c r="C18" s="1">
         <v>4723</v>
       </c>
       <c r="D18" s="1">
-        <v>0.23000000417232513</v>
+        <v>1.7400000095367432</v>
       </c>
       <c r="E18" s="1">
-        <v>2.5895299911499023</v>
+        <v>35.462589263916016</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B19" s="1">
-        <v>13.003781988992799</v>
+        <v>0</v>
       </c>
       <c r="C19" s="1">
         <v>4723</v>
       </c>
-      <c r="D19" s="1">
-        <v>0.34999999403953552</v>
-      </c>
-      <c r="E19" s="1">
-        <v>4.551323413848877</v>
-      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="1">
-        <v>16.457479089037886</v>
+        <v>0</v>
       </c>
       <c r="C20" s="1">
         <v>4723</v>
       </c>
       <c r="D20" s="1">
-        <v>0.40000000596046448</v>
+        <v>1.690000057220459</v>
       </c>
       <c r="E20" s="1">
-        <v>6.5829916000366211</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" s="1">
-        <v>8.7861950559533302</v>
+        <v>0</v>
       </c>
       <c r="C21" s="1">
         <v>4723</v>
       </c>
       <c r="D21" s="1">
-        <v>0.56499999761581421</v>
+        <v>1.4500000476837158</v>
       </c>
       <c r="E21" s="1">
-        <v>4.9642000198364258</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" s="1">
-        <v>20.343278355853879</v>
+        <v>0</v>
       </c>
       <c r="C22" s="1">
         <v>4723</v>
       </c>
       <c r="D22" s="1">
-        <v>1.3511111736297607</v>
+        <v>1.1100000143051147</v>
       </c>
       <c r="E22" s="1">
-        <v>27.486030578613281</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" s="1">
-        <v>8.6313793025682113</v>
+        <v>32.047278376572621</v>
       </c>
       <c r="C23" s="1">
         <v>4723</v>
       </c>
       <c r="D23" s="1">
-        <v>4.0584616661071777</v>
+        <v>0.85000002384185791</v>
       </c>
       <c r="E23" s="1">
-        <v>35.030120849609375</v>
+        <v>27.24018669128418</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" s="1">
-        <v>18.848436411321099</v>
+        <v>0</v>
       </c>
       <c r="C24" s="1">
         <v>4723</v>
       </c>
       <c r="D24" s="1">
-        <v>2.5450000762939453</v>
+        <v>2.7300000190734863</v>
       </c>
       <c r="E24" s="1">
-        <v>47.969272613525391</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="B25" s="1">
-        <v>45.674628638373122</v>
+        <v>0</v>
       </c>
       <c r="C25" s="1">
         <v>4723</v>
       </c>
-      <c r="D25" s="1">
-        <v>1.8233332633972168</v>
-      </c>
-      <c r="E25" s="1">
-        <v>83.280067443847656</v>
-      </c>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B26" s="1">
-        <v>15.668787100091466</v>
+        <v>0</v>
       </c>
       <c r="C26" s="1">
         <v>4723</v>
       </c>
       <c r="D26" s="1">
-        <v>1.2246154546737671</v>
+        <v>0.44499999284744263</v>
       </c>
       <c r="E26" s="1">
-        <v>19.188238143920898</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B27" s="1">
-        <v>39.989490301458105</v>
+        <v>7.5887418317259705</v>
       </c>
       <c r="C27" s="1">
         <v>4723</v>
       </c>
       <c r="D27" s="1">
-        <v>3.934999942779541</v>
+        <v>4.2849998474121094</v>
       </c>
       <c r="E27" s="1">
-        <v>157.358642578125</v>
+        <v>32.517757415771484</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B28" s="1">
-        <v>12.596166011213423</v>
+        <v>0</v>
       </c>
       <c r="C28" s="1">
         <v>4723</v>
       </c>
       <c r="D28" s="1">
-        <v>0.05000000074505806</v>
+        <v>0.87999999523162842</v>
       </c>
       <c r="E28" s="1">
-        <v>0.62980830669403076</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="1">
+        <v>26.284929443713143</v>
+      </c>
+      <c r="C29" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D29" s="1">
+        <v>3.684999942779541</v>
+      </c>
+      <c r="E29" s="1">
+        <v>96.859962463378906</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" s="1">
+        <v>0</v>
+      </c>
+      <c r="C30" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D30" s="1">
+        <v>2.9300000667572021</v>
+      </c>
+      <c r="E30" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B31" s="1">
+        <v>0</v>
+      </c>
+      <c r="C31" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D31" s="1">
+        <v>1.75</v>
+      </c>
+      <c r="E31" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="1">
+        <v>21.167612287823033</v>
+      </c>
+      <c r="C32" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D32" s="1">
+        <v>1.4500000476837158</v>
+      </c>
+      <c r="E32" s="1">
+        <v>30.693038940429688</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" s="1">
+        <v>0</v>
+      </c>
+      <c r="C33" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>30</v>
+      </c>
+      <c r="B34" s="1">
+        <v>25.771581386954455</v>
+      </c>
+      <c r="C34" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D34" s="1">
+        <v>9</v>
+      </c>
+      <c r="E34" s="1">
+        <v>231.94422912597656</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35" s="1">
+        <v>7.1381170796358608</v>
+      </c>
+      <c r="C35" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D35" s="1">
+        <v>5.8400001525878906</v>
+      </c>
+      <c r="E35" s="1">
+        <v>41.686603546142578</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>32</v>
+      </c>
+      <c r="B36" s="1">
+        <v>10.352916163835843</v>
+      </c>
+      <c r="C36" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D36" s="1">
+        <v>3.0799999237060547</v>
+      </c>
+      <c r="E36" s="1">
+        <v>31.886980056762695</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>9</v>
+      </c>
+      <c r="B37" s="1">
+        <v>0</v>
+      </c>
+      <c r="C37" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>33</v>
+      </c>
+      <c r="B38" s="1">
+        <v>39.938503641358324</v>
+      </c>
+      <c r="C38" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D38" s="1">
+        <v>1.1337499618530273</v>
+      </c>
+      <c r="E38" s="1">
+        <v>45.280277252197266</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B39" s="1">
+        <v>0</v>
+      </c>
+      <c r="C39" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D39" s="1">
+        <v>0.79000002145767212</v>
+      </c>
+      <c r="E39" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>35</v>
+      </c>
+      <c r="B40" s="1">
+        <v>21.064435758960215</v>
+      </c>
+      <c r="C40" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D40" s="1">
+        <v>1.6485714912414551</v>
+      </c>
+      <c r="E40" s="1">
+        <v>34.726226806640625</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>36</v>
+      </c>
+      <c r="B41" s="1">
+        <v>0</v>
+      </c>
+      <c r="C41" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D41" s="1">
+        <v>0.31000000238418579</v>
+      </c>
+      <c r="E41" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>37</v>
+      </c>
+      <c r="B42" s="1">
+        <v>0</v>
+      </c>
+      <c r="C42" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D42" s="1">
+        <v>0.70999997854232788</v>
+      </c>
+      <c r="E42" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>9</v>
+      </c>
+      <c r="B43" s="1">
+        <v>0</v>
+      </c>
+      <c r="C43" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>38</v>
+      </c>
+      <c r="B44" s="1">
+        <v>11.258825547660328</v>
+      </c>
+      <c r="C44" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D44" s="1">
+        <v>0.23000000417232513</v>
+      </c>
+      <c r="E44" s="1">
+        <v>2.5895299911499023</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>39</v>
+      </c>
+      <c r="B45" s="1">
+        <v>0</v>
+      </c>
+      <c r="C45" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D45" s="1">
+        <v>2</v>
+      </c>
+      <c r="E45" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>40</v>
+      </c>
+      <c r="B46" s="1">
+        <v>13.003781988992799</v>
+      </c>
+      <c r="C46" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D46" s="1">
+        <v>0.34999999403953552</v>
+      </c>
+      <c r="E46" s="1">
+        <v>4.551323413848877</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>41</v>
+      </c>
+      <c r="B47" s="1">
+        <v>16.457479089037886</v>
+      </c>
+      <c r="C47" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D47" s="1">
+        <v>0.40000000596046448</v>
+      </c>
+      <c r="E47" s="1">
+        <v>6.5829916000366211</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>42</v>
+      </c>
+      <c r="B48" s="1">
+        <v>0</v>
+      </c>
+      <c r="C48" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D48" s="1">
+        <v>0.38999998569488525</v>
+      </c>
+      <c r="E48" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>43</v>
+      </c>
+      <c r="B49" s="1">
+        <v>0</v>
+      </c>
+      <c r="C49" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D49" s="1">
+        <v>0.18000000715255737</v>
+      </c>
+      <c r="E49" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>44</v>
+      </c>
+      <c r="B50" s="1">
+        <v>0</v>
+      </c>
+      <c r="C50" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D50" s="1">
+        <v>0.37000000476837158</v>
+      </c>
+      <c r="E50" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>45</v>
+      </c>
+      <c r="B51" s="1">
+        <v>0</v>
+      </c>
+      <c r="C51" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D51" s="1">
+        <v>0.4699999988079071</v>
+      </c>
+      <c r="E51" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>46</v>
+      </c>
+      <c r="B52" s="1">
+        <v>8.7861950559533302</v>
+      </c>
+      <c r="C52" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D52" s="1">
+        <v>0.56499999761581421</v>
+      </c>
+      <c r="E52" s="1">
+        <v>4.9642000198364258</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>9</v>
+      </c>
+      <c r="B53" s="1">
+        <v>0</v>
+      </c>
+      <c r="C53" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>47</v>
+      </c>
+      <c r="B54" s="1">
+        <v>20.343278355853879</v>
+      </c>
+      <c r="C54" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D54" s="1">
+        <v>1.3511111736297607</v>
+      </c>
+      <c r="E54" s="1">
+        <v>27.486030578613281</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>48</v>
+      </c>
+      <c r="B55" s="1">
+        <v>8.6313793025682113</v>
+      </c>
+      <c r="C55" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D55" s="1">
+        <v>4.0584616661071777</v>
+      </c>
+      <c r="E55" s="1">
+        <v>35.030120849609375</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>49</v>
+      </c>
+      <c r="B56" s="1">
+        <v>18.848436411321099</v>
+      </c>
+      <c r="C56" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D56" s="1">
+        <v>2.5450000762939453</v>
+      </c>
+      <c r="E56" s="1">
+        <v>47.969272613525391</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>50</v>
+      </c>
+      <c r="B57" s="1">
+        <v>0</v>
+      </c>
+      <c r="C57" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D57" s="1">
+        <v>2.9000000953674316</v>
+      </c>
+      <c r="E57" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>9</v>
+      </c>
+      <c r="B58" s="1">
+        <v>0</v>
+      </c>
+      <c r="C58" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>51</v>
+      </c>
+      <c r="B59" s="1">
+        <v>0</v>
+      </c>
+      <c r="C59" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D59" s="1">
+        <v>7.2100000381469727</v>
+      </c>
+      <c r="E59" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>52</v>
+      </c>
+      <c r="B60" s="1">
+        <v>0</v>
+      </c>
+      <c r="C60" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D60" s="1">
+        <v>6.3449997901916504</v>
+      </c>
+      <c r="E60" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>53</v>
+      </c>
+      <c r="B61" s="1">
+        <v>0</v>
+      </c>
+      <c r="C61" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D61" s="1">
+        <v>5.6700000762939453</v>
+      </c>
+      <c r="E61" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>9</v>
+      </c>
+      <c r="B62" s="1">
+        <v>0</v>
+      </c>
+      <c r="C62" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>54</v>
+      </c>
+      <c r="B63" s="1">
+        <v>45.674628638373122</v>
+      </c>
+      <c r="C63" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D63" s="1">
+        <v>1.8233332633972168</v>
+      </c>
+      <c r="E63" s="1">
+        <v>83.280067443847656</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>55</v>
+      </c>
+      <c r="B64" s="1">
+        <v>15.668787100091466</v>
+      </c>
+      <c r="C64" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D64" s="1">
+        <v>1.2246154546737671</v>
+      </c>
+      <c r="E64" s="1">
+        <v>19.188238143920898</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>56</v>
+      </c>
+      <c r="B65" s="1">
+        <v>0</v>
+      </c>
+      <c r="C65" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D65" s="1">
+        <v>1.2000000476837158</v>
+      </c>
+      <c r="E65" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>57</v>
+      </c>
+      <c r="B66" s="1">
+        <v>0</v>
+      </c>
+      <c r="C66" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D66" s="1">
+        <v>0.25999999046325684</v>
+      </c>
+      <c r="E66" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>58</v>
+      </c>
+      <c r="B67" s="1">
+        <v>0</v>
+      </c>
+      <c r="C67" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D67" s="1">
+        <v>3.3299999237060547</v>
+      </c>
+      <c r="E67" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s">
+        <v>9</v>
+      </c>
+      <c r="B68" s="1">
+        <v>0</v>
+      </c>
+      <c r="C68" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+    </row>
+    <row r="69">
+      <c r="A69" t="s">
+        <v>59</v>
+      </c>
+      <c r="B69" s="1">
+        <v>39.989490301458105</v>
+      </c>
+      <c r="C69" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D69" s="1">
+        <v>3.934999942779541</v>
+      </c>
+      <c r="E69" s="1">
+        <v>157.358642578125</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s">
+        <v>60</v>
+      </c>
+      <c r="B70" s="1">
+        <v>0</v>
+      </c>
+      <c r="C70" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D70" s="1">
+        <v>3.6700000762939453</v>
+      </c>
+      <c r="E70" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s">
+        <v>61</v>
+      </c>
+      <c r="B71" s="1">
+        <v>0</v>
+      </c>
+      <c r="C71" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D71" s="1">
+        <v>3.5999999046325684</v>
+      </c>
+      <c r="E71" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s">
+        <v>62</v>
+      </c>
+      <c r="B72" s="1">
+        <v>0</v>
+      </c>
+      <c r="C72" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D72" s="1">
+        <v>3.3199999332427979</v>
+      </c>
+      <c r="E72" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s">
+        <v>63</v>
+      </c>
+      <c r="B73" s="1">
+        <v>0</v>
+      </c>
+      <c r="C73" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D73" s="1">
+        <v>3.6400001049041748</v>
+      </c>
+      <c r="E73" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s">
+        <v>9</v>
+      </c>
+      <c r="B74" s="1">
+        <v>0</v>
+      </c>
+      <c r="C74" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D74" s="1"/>
+      <c r="E74" s="1"/>
+    </row>
+    <row r="75">
+      <c r="A75" t="s">
+        <v>64</v>
+      </c>
+      <c r="B75" s="1">
+        <v>12.596166011213423</v>
+      </c>
+      <c r="C75" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D75" s="1">
+        <v>0.05000000074505806</v>
+      </c>
+      <c r="E75" s="1">
+        <v>0.62980830669403076</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s">
+        <v>65</v>
+      </c>
+      <c r="B76" s="1">
+        <v>0</v>
+      </c>
+      <c r="C76" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D76" s="1">
+        <v>0.039999999105930328</v>
+      </c>
+      <c r="E76" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s">
+        <v>66</v>
+      </c>
+      <c r="B77" s="1">
+        <v>0</v>
+      </c>
+      <c r="C77" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D77" s="1">
+        <v>0.88999998569488525</v>
+      </c>
+      <c r="E77" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s">
+        <v>9</v>
+      </c>
+      <c r="B78" s="1">
+        <v>0</v>
+      </c>
+      <c r="C78" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D78" s="1"/>
+      <c r="E78" s="1"/>
+    </row>
+    <row r="79">
+      <c r="A79" t="s">
+        <v>67</v>
+      </c>
+      <c r="B79" s="1">
         <v>22.535818373730393</v>
       </c>
-      <c r="C29" s="1">
-        <v>4723</v>
-      </c>
-      <c r="D29" s="1">
-        <v>0</v>
-      </c>
-      <c r="E29" s="1">
-        <v>0</v>
-      </c>
+      <c r="C79" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D79" s="1">
+        <v>0</v>
+      </c>
+      <c r="E79" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s">
+        <v>68</v>
+      </c>
+      <c r="B80" s="1">
+        <v>0</v>
+      </c>
+      <c r="C80" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D80" s="1">
+        <v>3.1520001888275146</v>
+      </c>
+      <c r="E80" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s">
+        <v>69</v>
+      </c>
+      <c r="B81" s="1">
+        <v>0</v>
+      </c>
+      <c r="C81" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D81" s="1">
+        <v>1.0900000333786011</v>
+      </c>
+      <c r="E81" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s">
+        <v>70</v>
+      </c>
+      <c r="B82" s="1">
+        <v>0</v>
+      </c>
+      <c r="C82" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D82" s="1">
+        <v>0.93999999761581421</v>
+      </c>
+      <c r="E82" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s">
+        <v>9</v>
+      </c>
+      <c r="B83" s="1">
+        <v>0</v>
+      </c>
+      <c r="C83" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D83" s="1"/>
+      <c r="E83" s="1"/>
+    </row>
+    <row r="84">
+      <c r="A84" t="s">
+        <v>71</v>
+      </c>
+      <c r="B84" s="1">
+        <v>0</v>
+      </c>
+      <c r="C84" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D84" s="1">
+        <v>0.43666666746139526</v>
+      </c>
+      <c r="E84" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s">
+        <v>72</v>
+      </c>
+      <c r="B85" s="1">
+        <v>0</v>
+      </c>
+      <c r="C85" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D85" s="1">
+        <v>0</v>
+      </c>
+      <c r="E85" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s">
+        <v>73</v>
+      </c>
+      <c r="B86" s="1">
+        <v>0</v>
+      </c>
+      <c r="C86" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D86" s="1">
+        <v>0.43999999761581421</v>
+      </c>
+      <c r="E86" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s">
+        <v>74</v>
+      </c>
+      <c r="B87" s="1">
+        <v>0</v>
+      </c>
+      <c r="C87" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D87" s="1">
+        <v>0.4050000011920929</v>
+      </c>
+      <c r="E87" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s">
+        <v>75</v>
+      </c>
+      <c r="B88" s="1">
+        <v>0</v>
+      </c>
+      <c r="C88" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D88" s="1">
+        <v>1.8069999217987061</v>
+      </c>
+      <c r="E88" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s">
+        <v>9</v>
+      </c>
+      <c r="B89" s="1">
+        <v>0</v>
+      </c>
+      <c r="C89" s="1">
+        <v>4723</v>
+      </c>
+      <c r="D89" s="1"/>
+      <c r="E89" s="1"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>